<commit_message>
headings added and parts updated after meeting
</commit_message>
<xml_diff>
--- a/Misc/Dissertation Metrics.xlsx
+++ b/Misc/Dissertation Metrics.xlsx
@@ -393,7 +393,7 @@
   <dimension ref="C3:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,9 +626,12 @@
       <c r="C10" s="1">
         <v>43256</v>
       </c>
+      <c r="D10">
+        <v>4374</v>
+      </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>-4084</v>
+        <v>290</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -637,9 +640,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H10">
+        <v>170</v>
+      </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="J10">
         <v>75</v>
@@ -658,7 +664,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-4374</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
@@ -666,7 +672,7 @@
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K11">
         <f t="shared" si="3"/>
@@ -687,7 +693,7 @@
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K12">
         <f t="shared" si="3"/>
@@ -708,7 +714,7 @@
       </c>
       <c r="I13">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K13">
         <f t="shared" si="3"/>
@@ -729,7 +735,7 @@
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K14">
         <f t="shared" si="3"/>
@@ -750,7 +756,7 @@
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K15">
         <f t="shared" si="3"/>
@@ -771,7 +777,7 @@
       </c>
       <c r="I16">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K16">
         <f t="shared" si="3"/>
@@ -792,7 +798,7 @@
       </c>
       <c r="I17">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K17">
         <f t="shared" si="3"/>
@@ -813,7 +819,7 @@
       </c>
       <c r="I18">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K18">
         <f t="shared" si="3"/>
@@ -834,7 +840,7 @@
       </c>
       <c r="I19">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K19">
         <f t="shared" si="3"/>
@@ -855,7 +861,7 @@
       </c>
       <c r="I20">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K20">
         <f t="shared" si="3"/>
@@ -876,7 +882,7 @@
       </c>
       <c r="I21">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K21">
         <f t="shared" si="3"/>
@@ -897,7 +903,7 @@
       </c>
       <c r="I22">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K22">
         <f t="shared" si="3"/>
@@ -918,7 +924,7 @@
       </c>
       <c r="I23">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K23">
         <f t="shared" si="3"/>
@@ -939,7 +945,7 @@
       </c>
       <c r="I24">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K24">
         <f t="shared" si="3"/>
@@ -960,7 +966,7 @@
       </c>
       <c r="I25">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K25">
         <f t="shared" si="3"/>
@@ -981,7 +987,7 @@
       </c>
       <c r="I26">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K26">
         <f t="shared" si="3"/>
@@ -1002,7 +1008,7 @@
       </c>
       <c r="I27">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K27">
         <f t="shared" si="3"/>
@@ -1023,7 +1029,7 @@
       </c>
       <c r="I28">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K28">
         <f t="shared" si="3"/>
@@ -1044,7 +1050,7 @@
       </c>
       <c r="I29">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K29">
         <f t="shared" si="3"/>
@@ -1065,7 +1071,7 @@
       </c>
       <c r="I30">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K30">
         <f t="shared" si="3"/>
@@ -1086,7 +1092,7 @@
       </c>
       <c r="I31">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K31">
         <f t="shared" si="3"/>
@@ -1107,7 +1113,7 @@
       </c>
       <c r="I32">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K32">
         <f t="shared" si="3"/>
@@ -1128,7 +1134,7 @@
       </c>
       <c r="I33">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K33">
         <f t="shared" si="3"/>
@@ -1149,7 +1155,7 @@
       </c>
       <c r="I34">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K34">
         <f t="shared" si="3"/>
@@ -1170,7 +1176,7 @@
       </c>
       <c r="I35">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K35">
         <f t="shared" si="3"/>
@@ -1191,7 +1197,7 @@
       </c>
       <c r="I36">
         <f t="shared" si="2"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K36">
         <f t="shared" si="3"/>
@@ -1212,7 +1218,7 @@
       </c>
       <c r="I37">
         <f t="shared" ref="I37:I68" si="6">I36+H37</f>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K37">
         <f t="shared" si="3"/>
@@ -1233,7 +1239,7 @@
       </c>
       <c r="I38">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K38">
         <f t="shared" ref="K38:K69" si="7">J38-J37</f>
@@ -1254,7 +1260,7 @@
       </c>
       <c r="I39">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K39">
         <f t="shared" si="7"/>
@@ -1275,7 +1281,7 @@
       </c>
       <c r="I40">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K40">
         <f t="shared" si="7"/>
@@ -1296,7 +1302,7 @@
       </c>
       <c r="I41">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K41">
         <f t="shared" si="7"/>
@@ -1317,7 +1323,7 @@
       </c>
       <c r="I42">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K42">
         <f t="shared" si="7"/>
@@ -1338,7 +1344,7 @@
       </c>
       <c r="I43">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K43">
         <f t="shared" si="7"/>
@@ -1359,7 +1365,7 @@
       </c>
       <c r="I44">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K44">
         <f t="shared" si="7"/>
@@ -1380,7 +1386,7 @@
       </c>
       <c r="I45">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K45">
         <f t="shared" si="7"/>
@@ -1401,7 +1407,7 @@
       </c>
       <c r="I46">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K46">
         <f t="shared" si="7"/>
@@ -1422,7 +1428,7 @@
       </c>
       <c r="I47">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K47">
         <f t="shared" si="7"/>
@@ -1443,7 +1449,7 @@
       </c>
       <c r="I48">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K48">
         <f t="shared" si="7"/>
@@ -1464,7 +1470,7 @@
       </c>
       <c r="I49">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K49">
         <f t="shared" si="7"/>
@@ -1485,7 +1491,7 @@
       </c>
       <c r="I50">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K50">
         <f t="shared" si="7"/>
@@ -1506,7 +1512,7 @@
       </c>
       <c r="I51">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K51">
         <f t="shared" si="7"/>
@@ -1527,7 +1533,7 @@
       </c>
       <c r="I52">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K52">
         <f t="shared" si="7"/>
@@ -1548,7 +1554,7 @@
       </c>
       <c r="I53">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K53">
         <f t="shared" si="7"/>
@@ -1569,7 +1575,7 @@
       </c>
       <c r="I54">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K54">
         <f t="shared" si="7"/>
@@ -1590,7 +1596,7 @@
       </c>
       <c r="I55">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K55">
         <f t="shared" si="7"/>
@@ -1611,7 +1617,7 @@
       </c>
       <c r="I56">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K56">
         <f t="shared" si="7"/>
@@ -1632,7 +1638,7 @@
       </c>
       <c r="I57">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K57">
         <f t="shared" si="7"/>
@@ -1653,7 +1659,7 @@
       </c>
       <c r="I58">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K58">
         <f t="shared" si="7"/>
@@ -1674,7 +1680,7 @@
       </c>
       <c r="I59">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K59">
         <f t="shared" si="7"/>
@@ -1695,7 +1701,7 @@
       </c>
       <c r="I60">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K60">
         <f t="shared" si="7"/>
@@ -1716,7 +1722,7 @@
       </c>
       <c r="I61">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K61">
         <f t="shared" si="7"/>
@@ -1737,7 +1743,7 @@
       </c>
       <c r="I62">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K62">
         <f t="shared" si="7"/>
@@ -1758,7 +1764,7 @@
       </c>
       <c r="I63">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K63">
         <f t="shared" si="7"/>
@@ -1779,7 +1785,7 @@
       </c>
       <c r="I64">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K64">
         <f t="shared" si="7"/>
@@ -1800,7 +1806,7 @@
       </c>
       <c r="I65">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K65">
         <f t="shared" si="7"/>
@@ -1821,7 +1827,7 @@
       </c>
       <c r="I66">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K66">
         <f t="shared" si="7"/>
@@ -1842,7 +1848,7 @@
       </c>
       <c r="I67">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K67">
         <f t="shared" si="7"/>
@@ -1863,7 +1869,7 @@
       </c>
       <c r="I68">
         <f t="shared" si="6"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K68">
         <f t="shared" si="7"/>
@@ -1884,7 +1890,7 @@
       </c>
       <c r="I69">
         <f t="shared" ref="I69:I100" si="10">I68+H69</f>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K69">
         <f t="shared" si="7"/>
@@ -1905,7 +1911,7 @@
       </c>
       <c r="I70">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K70">
         <f t="shared" ref="K70:K101" si="11">J70-J69</f>
@@ -1926,7 +1932,7 @@
       </c>
       <c r="I71">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K71">
         <f t="shared" si="11"/>
@@ -1947,7 +1953,7 @@
       </c>
       <c r="I72">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K72">
         <f t="shared" si="11"/>
@@ -1968,7 +1974,7 @@
       </c>
       <c r="I73">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K73">
         <f t="shared" si="11"/>
@@ -1989,7 +1995,7 @@
       </c>
       <c r="I74">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K74">
         <f t="shared" si="11"/>
@@ -2010,7 +2016,7 @@
       </c>
       <c r="I75">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K75">
         <f t="shared" si="11"/>
@@ -2031,7 +2037,7 @@
       </c>
       <c r="I76">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K76">
         <f t="shared" si="11"/>
@@ -2052,7 +2058,7 @@
       </c>
       <c r="I77">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K77">
         <f t="shared" si="11"/>
@@ -2073,7 +2079,7 @@
       </c>
       <c r="I78">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K78">
         <f t="shared" si="11"/>
@@ -2094,7 +2100,7 @@
       </c>
       <c r="I79">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K79">
         <f t="shared" si="11"/>
@@ -2115,7 +2121,7 @@
       </c>
       <c r="I80">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K80">
         <f t="shared" si="11"/>
@@ -2136,7 +2142,7 @@
       </c>
       <c r="I81">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K81">
         <f t="shared" si="11"/>
@@ -2157,7 +2163,7 @@
       </c>
       <c r="I82">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K82">
         <f t="shared" si="11"/>
@@ -2178,7 +2184,7 @@
       </c>
       <c r="I83">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K83">
         <f t="shared" si="11"/>
@@ -2199,7 +2205,7 @@
       </c>
       <c r="I84">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K84">
         <f t="shared" si="11"/>
@@ -2220,7 +2226,7 @@
       </c>
       <c r="I85">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K85">
         <f t="shared" si="11"/>
@@ -2241,7 +2247,7 @@
       </c>
       <c r="I86">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K86">
         <f t="shared" si="11"/>
@@ -2262,7 +2268,7 @@
       </c>
       <c r="I87">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K87">
         <f t="shared" si="11"/>
@@ -2283,7 +2289,7 @@
       </c>
       <c r="I88">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K88">
         <f t="shared" si="11"/>
@@ -2304,7 +2310,7 @@
       </c>
       <c r="I89">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K89">
         <f t="shared" si="11"/>
@@ -2325,7 +2331,7 @@
       </c>
       <c r="I90">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K90">
         <f t="shared" si="11"/>
@@ -2346,7 +2352,7 @@
       </c>
       <c r="I91">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K91">
         <f t="shared" si="11"/>
@@ -2367,7 +2373,7 @@
       </c>
       <c r="I92">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K92">
         <f t="shared" si="11"/>
@@ -2388,7 +2394,7 @@
       </c>
       <c r="I93">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K93">
         <f t="shared" si="11"/>
@@ -2409,7 +2415,7 @@
       </c>
       <c r="I94">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K94">
         <f t="shared" si="11"/>
@@ -2430,7 +2436,7 @@
       </c>
       <c r="I95">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K95">
         <f t="shared" si="11"/>
@@ -2451,7 +2457,7 @@
       </c>
       <c r="I96">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K96">
         <f t="shared" si="11"/>
@@ -2472,7 +2478,7 @@
       </c>
       <c r="I97">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K97">
         <f t="shared" si="11"/>
@@ -2493,7 +2499,7 @@
       </c>
       <c r="I98">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K98">
         <f t="shared" si="11"/>
@@ -2514,7 +2520,7 @@
       </c>
       <c r="I99">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K99">
         <f t="shared" si="11"/>
@@ -2535,7 +2541,7 @@
       </c>
       <c r="I100">
         <f t="shared" si="10"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K100">
         <f t="shared" si="11"/>
@@ -2556,7 +2562,7 @@
       </c>
       <c r="I101">
         <f t="shared" ref="I101:I118" si="14">I100+H101</f>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K101">
         <f t="shared" si="11"/>
@@ -2577,7 +2583,7 @@
       </c>
       <c r="I102">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K102">
         <f t="shared" ref="K102:K118" si="15">J102-J101</f>
@@ -2598,7 +2604,7 @@
       </c>
       <c r="I103">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K103">
         <f t="shared" si="15"/>
@@ -2619,7 +2625,7 @@
       </c>
       <c r="I104">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K104">
         <f t="shared" si="15"/>
@@ -2640,7 +2646,7 @@
       </c>
       <c r="I105">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K105">
         <f t="shared" si="15"/>
@@ -2661,7 +2667,7 @@
       </c>
       <c r="I106">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K106">
         <f t="shared" si="15"/>
@@ -2682,7 +2688,7 @@
       </c>
       <c r="I107">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K107">
         <f t="shared" si="15"/>
@@ -2703,7 +2709,7 @@
       </c>
       <c r="I108">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K108">
         <f t="shared" si="15"/>
@@ -2724,7 +2730,7 @@
       </c>
       <c r="I109">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K109">
         <f t="shared" si="15"/>
@@ -2745,7 +2751,7 @@
       </c>
       <c r="I110">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K110">
         <f t="shared" si="15"/>
@@ -2766,7 +2772,7 @@
       </c>
       <c r="I111">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K111">
         <f t="shared" si="15"/>
@@ -2787,7 +2793,7 @@
       </c>
       <c r="I112">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K112">
         <f t="shared" si="15"/>
@@ -2808,7 +2814,7 @@
       </c>
       <c r="I113">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K113">
         <f t="shared" si="15"/>
@@ -2829,7 +2835,7 @@
       </c>
       <c r="I114">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K114">
         <f t="shared" si="15"/>
@@ -2850,7 +2856,7 @@
       </c>
       <c r="I115">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K115">
         <f t="shared" si="15"/>
@@ -2871,7 +2877,7 @@
       </c>
       <c r="I116">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K116">
         <f t="shared" si="15"/>
@@ -2892,7 +2898,7 @@
       </c>
       <c r="I117">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K117">
         <f t="shared" si="15"/>
@@ -2913,7 +2919,7 @@
       </c>
       <c r="I118">
         <f t="shared" si="14"/>
-        <v>1139</v>
+        <v>1309</v>
       </c>
       <c r="K118">
         <f t="shared" si="15"/>

</xml_diff>

<commit_message>
literally just added headings
</commit_message>
<xml_diff>
--- a/Misc/Dissertation Metrics.xlsx
+++ b/Misc/Dissertation Metrics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\483446\Documents\Semester-2\MSc-Dissertation\Misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\483446\Documents\Trimester-3\MSc-Dissertation\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>250 Miles by Radio Moscow</t>
+  </si>
+  <si>
+    <t>Return Trip by Electric Wizard</t>
   </si>
 </sst>
 </file>
@@ -393,7 +396,7 @@
   <dimension ref="C3:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,21 +665,36 @@
       <c r="C11" s="1">
         <v>43257</v>
       </c>
+      <c r="D11">
+        <v>4385</v>
+      </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>-4374</v>
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H11">
+        <v>329</v>
+      </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
+      </c>
+      <c r="J11">
+        <v>50</v>
       </c>
       <c r="K11">
         <f t="shared" si="3"/>
-        <v>-75</v>
+        <v>-25</v>
+      </c>
+      <c r="L11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.25">
@@ -685,7 +703,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-4385</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
@@ -693,11 +711,11 @@
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.25">
@@ -714,7 +732,7 @@
       </c>
       <c r="I13">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K13">
         <f t="shared" si="3"/>
@@ -735,7 +753,7 @@
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K14">
         <f t="shared" si="3"/>
@@ -756,7 +774,7 @@
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K15">
         <f t="shared" si="3"/>
@@ -777,7 +795,7 @@
       </c>
       <c r="I16">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K16">
         <f t="shared" si="3"/>
@@ -798,7 +816,7 @@
       </c>
       <c r="I17">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K17">
         <f t="shared" si="3"/>
@@ -819,7 +837,7 @@
       </c>
       <c r="I18">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K18">
         <f t="shared" si="3"/>
@@ -840,7 +858,7 @@
       </c>
       <c r="I19">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K19">
         <f t="shared" si="3"/>
@@ -861,7 +879,7 @@
       </c>
       <c r="I20">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K20">
         <f t="shared" si="3"/>
@@ -882,7 +900,7 @@
       </c>
       <c r="I21">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K21">
         <f t="shared" si="3"/>
@@ -903,7 +921,7 @@
       </c>
       <c r="I22">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K22">
         <f t="shared" si="3"/>
@@ -924,7 +942,7 @@
       </c>
       <c r="I23">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K23">
         <f t="shared" si="3"/>
@@ -945,7 +963,7 @@
       </c>
       <c r="I24">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K24">
         <f t="shared" si="3"/>
@@ -966,7 +984,7 @@
       </c>
       <c r="I25">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K25">
         <f t="shared" si="3"/>
@@ -987,7 +1005,7 @@
       </c>
       <c r="I26">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K26">
         <f t="shared" si="3"/>
@@ -1008,7 +1026,7 @@
       </c>
       <c r="I27">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K27">
         <f t="shared" si="3"/>
@@ -1029,7 +1047,7 @@
       </c>
       <c r="I28">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K28">
         <f t="shared" si="3"/>
@@ -1050,7 +1068,7 @@
       </c>
       <c r="I29">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K29">
         <f t="shared" si="3"/>
@@ -1071,7 +1089,7 @@
       </c>
       <c r="I30">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K30">
         <f t="shared" si="3"/>
@@ -1092,7 +1110,7 @@
       </c>
       <c r="I31">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K31">
         <f t="shared" si="3"/>
@@ -1113,7 +1131,7 @@
       </c>
       <c r="I32">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K32">
         <f t="shared" si="3"/>
@@ -1134,7 +1152,7 @@
       </c>
       <c r="I33">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K33">
         <f t="shared" si="3"/>
@@ -1155,7 +1173,7 @@
       </c>
       <c r="I34">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K34">
         <f t="shared" si="3"/>
@@ -1176,7 +1194,7 @@
       </c>
       <c r="I35">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K35">
         <f t="shared" si="3"/>
@@ -1197,7 +1215,7 @@
       </c>
       <c r="I36">
         <f t="shared" si="2"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K36">
         <f t="shared" si="3"/>
@@ -1218,7 +1236,7 @@
       </c>
       <c r="I37">
         <f t="shared" ref="I37:I68" si="6">I36+H37</f>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K37">
         <f t="shared" si="3"/>
@@ -1239,7 +1257,7 @@
       </c>
       <c r="I38">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K38">
         <f t="shared" ref="K38:K69" si="7">J38-J37</f>
@@ -1260,7 +1278,7 @@
       </c>
       <c r="I39">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K39">
         <f t="shared" si="7"/>
@@ -1281,7 +1299,7 @@
       </c>
       <c r="I40">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K40">
         <f t="shared" si="7"/>
@@ -1302,7 +1320,7 @@
       </c>
       <c r="I41">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K41">
         <f t="shared" si="7"/>
@@ -1323,7 +1341,7 @@
       </c>
       <c r="I42">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K42">
         <f t="shared" si="7"/>
@@ -1344,7 +1362,7 @@
       </c>
       <c r="I43">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K43">
         <f t="shared" si="7"/>
@@ -1365,7 +1383,7 @@
       </c>
       <c r="I44">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K44">
         <f t="shared" si="7"/>
@@ -1386,7 +1404,7 @@
       </c>
       <c r="I45">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K45">
         <f t="shared" si="7"/>
@@ -1407,7 +1425,7 @@
       </c>
       <c r="I46">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K46">
         <f t="shared" si="7"/>
@@ -1428,7 +1446,7 @@
       </c>
       <c r="I47">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K47">
         <f t="shared" si="7"/>
@@ -1449,7 +1467,7 @@
       </c>
       <c r="I48">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K48">
         <f t="shared" si="7"/>
@@ -1470,7 +1488,7 @@
       </c>
       <c r="I49">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K49">
         <f t="shared" si="7"/>
@@ -1491,7 +1509,7 @@
       </c>
       <c r="I50">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K50">
         <f t="shared" si="7"/>
@@ -1512,7 +1530,7 @@
       </c>
       <c r="I51">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K51">
         <f t="shared" si="7"/>
@@ -1533,7 +1551,7 @@
       </c>
       <c r="I52">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K52">
         <f t="shared" si="7"/>
@@ -1554,7 +1572,7 @@
       </c>
       <c r="I53">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K53">
         <f t="shared" si="7"/>
@@ -1575,7 +1593,7 @@
       </c>
       <c r="I54">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K54">
         <f t="shared" si="7"/>
@@ -1596,7 +1614,7 @@
       </c>
       <c r="I55">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K55">
         <f t="shared" si="7"/>
@@ -1617,7 +1635,7 @@
       </c>
       <c r="I56">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K56">
         <f t="shared" si="7"/>
@@ -1638,7 +1656,7 @@
       </c>
       <c r="I57">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K57">
         <f t="shared" si="7"/>
@@ -1659,7 +1677,7 @@
       </c>
       <c r="I58">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K58">
         <f t="shared" si="7"/>
@@ -1680,7 +1698,7 @@
       </c>
       <c r="I59">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K59">
         <f t="shared" si="7"/>
@@ -1701,7 +1719,7 @@
       </c>
       <c r="I60">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K60">
         <f t="shared" si="7"/>
@@ -1722,7 +1740,7 @@
       </c>
       <c r="I61">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K61">
         <f t="shared" si="7"/>
@@ -1743,7 +1761,7 @@
       </c>
       <c r="I62">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K62">
         <f t="shared" si="7"/>
@@ -1764,7 +1782,7 @@
       </c>
       <c r="I63">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K63">
         <f t="shared" si="7"/>
@@ -1785,7 +1803,7 @@
       </c>
       <c r="I64">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K64">
         <f t="shared" si="7"/>
@@ -1806,7 +1824,7 @@
       </c>
       <c r="I65">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K65">
         <f t="shared" si="7"/>
@@ -1827,7 +1845,7 @@
       </c>
       <c r="I66">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K66">
         <f t="shared" si="7"/>
@@ -1848,7 +1866,7 @@
       </c>
       <c r="I67">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K67">
         <f t="shared" si="7"/>
@@ -1869,7 +1887,7 @@
       </c>
       <c r="I68">
         <f t="shared" si="6"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K68">
         <f t="shared" si="7"/>
@@ -1890,7 +1908,7 @@
       </c>
       <c r="I69">
         <f t="shared" ref="I69:I100" si="10">I68+H69</f>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K69">
         <f t="shared" si="7"/>
@@ -1911,7 +1929,7 @@
       </c>
       <c r="I70">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K70">
         <f t="shared" ref="K70:K101" si="11">J70-J69</f>
@@ -1932,7 +1950,7 @@
       </c>
       <c r="I71">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K71">
         <f t="shared" si="11"/>
@@ -1953,7 +1971,7 @@
       </c>
       <c r="I72">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K72">
         <f t="shared" si="11"/>
@@ -1974,7 +1992,7 @@
       </c>
       <c r="I73">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K73">
         <f t="shared" si="11"/>
@@ -1995,7 +2013,7 @@
       </c>
       <c r="I74">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K74">
         <f t="shared" si="11"/>
@@ -2016,7 +2034,7 @@
       </c>
       <c r="I75">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K75">
         <f t="shared" si="11"/>
@@ -2037,7 +2055,7 @@
       </c>
       <c r="I76">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K76">
         <f t="shared" si="11"/>
@@ -2058,7 +2076,7 @@
       </c>
       <c r="I77">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K77">
         <f t="shared" si="11"/>
@@ -2079,7 +2097,7 @@
       </c>
       <c r="I78">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K78">
         <f t="shared" si="11"/>
@@ -2100,7 +2118,7 @@
       </c>
       <c r="I79">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K79">
         <f t="shared" si="11"/>
@@ -2121,7 +2139,7 @@
       </c>
       <c r="I80">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K80">
         <f t="shared" si="11"/>
@@ -2142,7 +2160,7 @@
       </c>
       <c r="I81">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K81">
         <f t="shared" si="11"/>
@@ -2163,7 +2181,7 @@
       </c>
       <c r="I82">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K82">
         <f t="shared" si="11"/>
@@ -2184,7 +2202,7 @@
       </c>
       <c r="I83">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K83">
         <f t="shared" si="11"/>
@@ -2205,7 +2223,7 @@
       </c>
       <c r="I84">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K84">
         <f t="shared" si="11"/>
@@ -2226,7 +2244,7 @@
       </c>
       <c r="I85">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K85">
         <f t="shared" si="11"/>
@@ -2247,7 +2265,7 @@
       </c>
       <c r="I86">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K86">
         <f t="shared" si="11"/>
@@ -2268,7 +2286,7 @@
       </c>
       <c r="I87">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K87">
         <f t="shared" si="11"/>
@@ -2289,7 +2307,7 @@
       </c>
       <c r="I88">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K88">
         <f t="shared" si="11"/>
@@ -2310,7 +2328,7 @@
       </c>
       <c r="I89">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K89">
         <f t="shared" si="11"/>
@@ -2331,7 +2349,7 @@
       </c>
       <c r="I90">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K90">
         <f t="shared" si="11"/>
@@ -2352,7 +2370,7 @@
       </c>
       <c r="I91">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K91">
         <f t="shared" si="11"/>
@@ -2373,7 +2391,7 @@
       </c>
       <c r="I92">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K92">
         <f t="shared" si="11"/>
@@ -2394,7 +2412,7 @@
       </c>
       <c r="I93">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K93">
         <f t="shared" si="11"/>
@@ -2415,7 +2433,7 @@
       </c>
       <c r="I94">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K94">
         <f t="shared" si="11"/>
@@ -2436,7 +2454,7 @@
       </c>
       <c r="I95">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K95">
         <f t="shared" si="11"/>
@@ -2457,7 +2475,7 @@
       </c>
       <c r="I96">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K96">
         <f t="shared" si="11"/>
@@ -2478,7 +2496,7 @@
       </c>
       <c r="I97">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K97">
         <f t="shared" si="11"/>
@@ -2499,7 +2517,7 @@
       </c>
       <c r="I98">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K98">
         <f t="shared" si="11"/>
@@ -2520,7 +2538,7 @@
       </c>
       <c r="I99">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K99">
         <f t="shared" si="11"/>
@@ -2541,7 +2559,7 @@
       </c>
       <c r="I100">
         <f t="shared" si="10"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K100">
         <f t="shared" si="11"/>
@@ -2562,7 +2580,7 @@
       </c>
       <c r="I101">
         <f t="shared" ref="I101:I118" si="14">I100+H101</f>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K101">
         <f t="shared" si="11"/>
@@ -2583,7 +2601,7 @@
       </c>
       <c r="I102">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K102">
         <f t="shared" ref="K102:K118" si="15">J102-J101</f>
@@ -2604,7 +2622,7 @@
       </c>
       <c r="I103">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K103">
         <f t="shared" si="15"/>
@@ -2625,7 +2643,7 @@
       </c>
       <c r="I104">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K104">
         <f t="shared" si="15"/>
@@ -2646,7 +2664,7 @@
       </c>
       <c r="I105">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K105">
         <f t="shared" si="15"/>
@@ -2667,7 +2685,7 @@
       </c>
       <c r="I106">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K106">
         <f t="shared" si="15"/>
@@ -2688,7 +2706,7 @@
       </c>
       <c r="I107">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K107">
         <f t="shared" si="15"/>
@@ -2709,7 +2727,7 @@
       </c>
       <c r="I108">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K108">
         <f t="shared" si="15"/>
@@ -2730,7 +2748,7 @@
       </c>
       <c r="I109">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K109">
         <f t="shared" si="15"/>
@@ -2751,7 +2769,7 @@
       </c>
       <c r="I110">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K110">
         <f t="shared" si="15"/>
@@ -2772,7 +2790,7 @@
       </c>
       <c r="I111">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K111">
         <f t="shared" si="15"/>
@@ -2793,7 +2811,7 @@
       </c>
       <c r="I112">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K112">
         <f t="shared" si="15"/>
@@ -2814,7 +2832,7 @@
       </c>
       <c r="I113">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K113">
         <f t="shared" si="15"/>
@@ -2835,7 +2853,7 @@
       </c>
       <c r="I114">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K114">
         <f t="shared" si="15"/>
@@ -2856,7 +2874,7 @@
       </c>
       <c r="I115">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K115">
         <f t="shared" si="15"/>
@@ -2877,7 +2895,7 @@
       </c>
       <c r="I116">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K116">
         <f t="shared" si="15"/>
@@ -2898,7 +2916,7 @@
       </c>
       <c r="I117">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K117">
         <f t="shared" si="15"/>
@@ -2919,7 +2937,7 @@
       </c>
       <c r="I118">
         <f t="shared" si="14"/>
-        <v>1309</v>
+        <v>1638</v>
       </c>
       <c r="K118">
         <f t="shared" si="15"/>
@@ -2928,6 +2946,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improved time tplan to gantt chart, moved to open source, lost words!
</commit_message>
<xml_diff>
--- a/Misc/Dissertation Metrics.xlsx
+++ b/Misc/Dissertation Metrics.xlsx
@@ -102,13 +102,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -125,16 +124,135 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -142,8 +260,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -167,6 +300,57 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -178,14 +362,91 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -197,22 +458,22 @@
   <dimension ref="C3:L118"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="71.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="56.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="6.91"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -758,6 +1019,9 @@
         <f aca="false">D19 - D18</f>
         <v>-4975</v>
       </c>
+      <c r="F19" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="G19" s="0" t="n">
         <f aca="false">F19-F18</f>
         <v>0</v>
@@ -766,9 +1030,12 @@
         <f aca="false">I18+H19</f>
         <v>2160</v>
       </c>
+      <c r="J19" s="0" t="n">
+        <v>65</v>
+      </c>
       <c r="K19" s="0" t="n">
         <f aca="false">J19-J18</f>
-        <v>-60</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -789,7 +1056,7 @@
       </c>
       <c r="K20" s="0" t="n">
         <f aca="false">J20-J19</f>
-        <v>0</v>
+        <v>-65</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
linked library in subproject, added captions
</commit_message>
<xml_diff>
--- a/Misc/Dissertation Metrics.xlsx
+++ b/Misc/Dissertation Metrics.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -91,7 +91,16 @@
     <t xml:space="preserve">Stormy Monday by Stoned Jesus</t>
   </si>
   <si>
-    <t xml:space="preserve">Gimmie Shelter by The Rolling Stones</t>
+    <t xml:space="preserve">Gimme Shelter by The Rolling Stones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daydreaming by Radiohead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Chain by Fleetwood Mac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">News Of The World by The Jam</t>
   </si>
 </sst>
 </file>
@@ -457,22 +466,23 @@
   </sheetPr>
   <dimension ref="C3:L118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="56.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="6.91"/>
   </cols>
   <sheetData>
@@ -511,7 +521,7 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="1" t="n">
         <v>43251</v>
       </c>
@@ -543,7 +553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="1" t="n">
         <v>43252</v>
       </c>
@@ -1011,13 +1021,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="n">
         <v>43265</v>
       </c>
+      <c r="D19" s="0" t="n">
+        <v>4937</v>
+      </c>
       <c r="E19" s="0" t="n">
         <f aca="false">D19 - D18</f>
-        <v>-4975</v>
+        <v>-38</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>0</v>
@@ -1026,9 +1039,13 @@
         <f aca="false">F19-F18</f>
         <v>0</v>
       </c>
+      <c r="H19" s="0" t="n">
+        <f aca="false"> 419 + 141</f>
+        <v>560</v>
+      </c>
       <c r="I19" s="0" t="n">
         <f aca="false">I18+H19</f>
-        <v>2160</v>
+        <v>2720</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>65</v>
@@ -1037,68 +1054,111 @@
         <f aca="false">J19-J18</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L19" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="1" t="n">
         <v>43266</v>
       </c>
+      <c r="D20" s="0" t="n">
+        <v>5135</v>
+      </c>
       <c r="E20" s="0" t="n">
         <f aca="false">D20 - D19</f>
+        <v>198</v>
+      </c>
+      <c r="F20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="0" t="n">
         <f aca="false">F20-F19</f>
         <v>0</v>
       </c>
+      <c r="H20" s="0" t="n">
+        <v>390</v>
+      </c>
       <c r="I20" s="0" t="n">
         <f aca="false">I19+H20</f>
-        <v>2160</v>
+        <v>3110</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>100</v>
       </c>
       <c r="K20" s="0" t="n">
         <f aca="false">J20-J19</f>
-        <v>-65</v>
+        <v>35</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="n">
         <v>43267</v>
       </c>
+      <c r="D21" s="0" t="n">
+        <v>5206</v>
+      </c>
       <c r="E21" s="0" t="n">
         <f aca="false">D21 - D20</f>
-        <v>0</v>
+        <v>71</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <f aca="false"> 2616 - 3</f>
+        <v>2613</v>
       </c>
       <c r="G21" s="0" t="n">
         <f aca="false">F21-F20</f>
-        <v>0</v>
+        <v>2613</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>870</v>
       </c>
       <c r="I21" s="0" t="n">
         <f aca="false">I20+H21</f>
-        <v>2160</v>
+        <v>3980</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>80</v>
       </c>
       <c r="K21" s="0" t="n">
         <f aca="false">J21-J20</f>
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="1" t="n">
         <v>43268</v>
       </c>
+      <c r="D22" s="0" t="n">
+        <v>5315</v>
+      </c>
       <c r="E22" s="0" t="n">
         <f aca="false">D22 - D21</f>
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="G22" s="0" t="n">
         <f aca="false">F22-F21</f>
-        <v>0</v>
+        <v>-2613</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>77</v>
       </c>
       <c r="I22" s="0" t="n">
         <f aca="false">I21+H22</f>
-        <v>2160</v>
+        <v>4057</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>70</v>
       </c>
       <c r="K22" s="0" t="n">
         <f aca="false">J22-J21</f>
-        <v>0</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1107,7 +1167,7 @@
       </c>
       <c r="E23" s="0" t="n">
         <f aca="false">D23 - D22</f>
-        <v>0</v>
+        <v>-5315</v>
       </c>
       <c r="G23" s="0" t="n">
         <f aca="false">F23-F22</f>
@@ -1115,11 +1175,11 @@
       </c>
       <c r="I23" s="0" t="n">
         <f aca="false">I22+H23</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K23" s="0" t="n">
         <f aca="false">J23-J22</f>
-        <v>0</v>
+        <v>-70</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,7 +1196,7 @@
       </c>
       <c r="I24" s="0" t="n">
         <f aca="false">I23+H24</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K24" s="0" t="n">
         <f aca="false">J24-J23</f>
@@ -1157,7 +1217,7 @@
       </c>
       <c r="I25" s="0" t="n">
         <f aca="false">I24+H25</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K25" s="0" t="n">
         <f aca="false">J25-J24</f>
@@ -1178,7 +1238,7 @@
       </c>
       <c r="I26" s="0" t="n">
         <f aca="false">I25+H26</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K26" s="0" t="n">
         <f aca="false">J26-J25</f>
@@ -1199,7 +1259,7 @@
       </c>
       <c r="I27" s="0" t="n">
         <f aca="false">I26+H27</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K27" s="0" t="n">
         <f aca="false">J27-J26</f>
@@ -1220,7 +1280,7 @@
       </c>
       <c r="I28" s="0" t="n">
         <f aca="false">I27+H28</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K28" s="0" t="n">
         <f aca="false">J28-J27</f>
@@ -1241,7 +1301,7 @@
       </c>
       <c r="I29" s="0" t="n">
         <f aca="false">I28+H29</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K29" s="0" t="n">
         <f aca="false">J29-J28</f>
@@ -1262,7 +1322,7 @@
       </c>
       <c r="I30" s="0" t="n">
         <f aca="false">I29+H30</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K30" s="0" t="n">
         <f aca="false">J30-J29</f>
@@ -1283,7 +1343,7 @@
       </c>
       <c r="I31" s="0" t="n">
         <f aca="false">I30+H31</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K31" s="0" t="n">
         <f aca="false">J31-J30</f>
@@ -1304,7 +1364,7 @@
       </c>
       <c r="I32" s="0" t="n">
         <f aca="false">I31+H32</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K32" s="0" t="n">
         <f aca="false">J32-J31</f>
@@ -1325,7 +1385,7 @@
       </c>
       <c r="I33" s="0" t="n">
         <f aca="false">I32+H33</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K33" s="0" t="n">
         <f aca="false">J33-J32</f>
@@ -1346,7 +1406,7 @@
       </c>
       <c r="I34" s="0" t="n">
         <f aca="false">I33+H34</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K34" s="0" t="n">
         <f aca="false">J34-J33</f>
@@ -1367,7 +1427,7 @@
       </c>
       <c r="I35" s="0" t="n">
         <f aca="false">I34+H35</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K35" s="0" t="n">
         <f aca="false">J35-J34</f>
@@ -1388,7 +1448,7 @@
       </c>
       <c r="I36" s="0" t="n">
         <f aca="false">I35+H36</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K36" s="0" t="n">
         <f aca="false">J36-J35</f>
@@ -1409,7 +1469,7 @@
       </c>
       <c r="I37" s="0" t="n">
         <f aca="false">I36+H37</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K37" s="0" t="n">
         <f aca="false">J37-J36</f>
@@ -1430,7 +1490,7 @@
       </c>
       <c r="I38" s="0" t="n">
         <f aca="false">I37+H38</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K38" s="0" t="n">
         <f aca="false">J38-J37</f>
@@ -1451,7 +1511,7 @@
       </c>
       <c r="I39" s="0" t="n">
         <f aca="false">I38+H39</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K39" s="0" t="n">
         <f aca="false">J39-J38</f>
@@ -1472,7 +1532,7 @@
       </c>
       <c r="I40" s="0" t="n">
         <f aca="false">I39+H40</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K40" s="0" t="n">
         <f aca="false">J40-J39</f>
@@ -1493,7 +1553,7 @@
       </c>
       <c r="I41" s="0" t="n">
         <f aca="false">I40+H41</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K41" s="0" t="n">
         <f aca="false">J41-J40</f>
@@ -1514,7 +1574,7 @@
       </c>
       <c r="I42" s="0" t="n">
         <f aca="false">I41+H42</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K42" s="0" t="n">
         <f aca="false">J42-J41</f>
@@ -1535,7 +1595,7 @@
       </c>
       <c r="I43" s="0" t="n">
         <f aca="false">I42+H43</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K43" s="0" t="n">
         <f aca="false">J43-J42</f>
@@ -1556,7 +1616,7 @@
       </c>
       <c r="I44" s="0" t="n">
         <f aca="false">I43+H44</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K44" s="0" t="n">
         <f aca="false">J44-J43</f>
@@ -1577,7 +1637,7 @@
       </c>
       <c r="I45" s="0" t="n">
         <f aca="false">I44+H45</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K45" s="0" t="n">
         <f aca="false">J45-J44</f>
@@ -1598,7 +1658,7 @@
       </c>
       <c r="I46" s="0" t="n">
         <f aca="false">I45+H46</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K46" s="0" t="n">
         <f aca="false">J46-J45</f>
@@ -1619,7 +1679,7 @@
       </c>
       <c r="I47" s="0" t="n">
         <f aca="false">I46+H47</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K47" s="0" t="n">
         <f aca="false">J47-J46</f>
@@ -1640,7 +1700,7 @@
       </c>
       <c r="I48" s="0" t="n">
         <f aca="false">I47+H48</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K48" s="0" t="n">
         <f aca="false">J48-J47</f>
@@ -1661,7 +1721,7 @@
       </c>
       <c r="I49" s="0" t="n">
         <f aca="false">I48+H49</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K49" s="0" t="n">
         <f aca="false">J49-J48</f>
@@ -1682,7 +1742,7 @@
       </c>
       <c r="I50" s="0" t="n">
         <f aca="false">I49+H50</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K50" s="0" t="n">
         <f aca="false">J50-J49</f>
@@ -1703,7 +1763,7 @@
       </c>
       <c r="I51" s="0" t="n">
         <f aca="false">I50+H51</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K51" s="0" t="n">
         <f aca="false">J51-J50</f>
@@ -1724,7 +1784,7 @@
       </c>
       <c r="I52" s="0" t="n">
         <f aca="false">I51+H52</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K52" s="0" t="n">
         <f aca="false">J52-J51</f>
@@ -1745,7 +1805,7 @@
       </c>
       <c r="I53" s="0" t="n">
         <f aca="false">I52+H53</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K53" s="0" t="n">
         <f aca="false">J53-J52</f>
@@ -1766,7 +1826,7 @@
       </c>
       <c r="I54" s="0" t="n">
         <f aca="false">I53+H54</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K54" s="0" t="n">
         <f aca="false">J54-J53</f>
@@ -1787,7 +1847,7 @@
       </c>
       <c r="I55" s="0" t="n">
         <f aca="false">I54+H55</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K55" s="0" t="n">
         <f aca="false">J55-J54</f>
@@ -1808,7 +1868,7 @@
       </c>
       <c r="I56" s="0" t="n">
         <f aca="false">I55+H56</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K56" s="0" t="n">
         <f aca="false">J56-J55</f>
@@ -1829,7 +1889,7 @@
       </c>
       <c r="I57" s="0" t="n">
         <f aca="false">I56+H57</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K57" s="0" t="n">
         <f aca="false">J57-J56</f>
@@ -1850,7 +1910,7 @@
       </c>
       <c r="I58" s="0" t="n">
         <f aca="false">I57+H58</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K58" s="0" t="n">
         <f aca="false">J58-J57</f>
@@ -1871,7 +1931,7 @@
       </c>
       <c r="I59" s="0" t="n">
         <f aca="false">I58+H59</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K59" s="0" t="n">
         <f aca="false">J59-J58</f>
@@ -1892,7 +1952,7 @@
       </c>
       <c r="I60" s="0" t="n">
         <f aca="false">I59+H60</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K60" s="0" t="n">
         <f aca="false">J60-J59</f>
@@ -1913,7 +1973,7 @@
       </c>
       <c r="I61" s="0" t="n">
         <f aca="false">I60+H61</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K61" s="0" t="n">
         <f aca="false">J61-J60</f>
@@ -1934,7 +1994,7 @@
       </c>
       <c r="I62" s="0" t="n">
         <f aca="false">I61+H62</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K62" s="0" t="n">
         <f aca="false">J62-J61</f>
@@ -1955,7 +2015,7 @@
       </c>
       <c r="I63" s="0" t="n">
         <f aca="false">I62+H63</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K63" s="0" t="n">
         <f aca="false">J63-J62</f>
@@ -1976,7 +2036,7 @@
       </c>
       <c r="I64" s="0" t="n">
         <f aca="false">I63+H64</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K64" s="0" t="n">
         <f aca="false">J64-J63</f>
@@ -1997,7 +2057,7 @@
       </c>
       <c r="I65" s="0" t="n">
         <f aca="false">I64+H65</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K65" s="0" t="n">
         <f aca="false">J65-J64</f>
@@ -2018,7 +2078,7 @@
       </c>
       <c r="I66" s="0" t="n">
         <f aca="false">I65+H66</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K66" s="0" t="n">
         <f aca="false">J66-J65</f>
@@ -2039,7 +2099,7 @@
       </c>
       <c r="I67" s="0" t="n">
         <f aca="false">I66+H67</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K67" s="0" t="n">
         <f aca="false">J67-J66</f>
@@ -2060,7 +2120,7 @@
       </c>
       <c r="I68" s="0" t="n">
         <f aca="false">I67+H68</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K68" s="0" t="n">
         <f aca="false">J68-J67</f>
@@ -2081,7 +2141,7 @@
       </c>
       <c r="I69" s="0" t="n">
         <f aca="false">I68+H69</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K69" s="0" t="n">
         <f aca="false">J69-J68</f>
@@ -2102,7 +2162,7 @@
       </c>
       <c r="I70" s="0" t="n">
         <f aca="false">I69+H70</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K70" s="0" t="n">
         <f aca="false">J70-J69</f>
@@ -2123,7 +2183,7 @@
       </c>
       <c r="I71" s="0" t="n">
         <f aca="false">I70+H71</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K71" s="0" t="n">
         <f aca="false">J71-J70</f>
@@ -2144,7 +2204,7 @@
       </c>
       <c r="I72" s="0" t="n">
         <f aca="false">I71+H72</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K72" s="0" t="n">
         <f aca="false">J72-J71</f>
@@ -2165,7 +2225,7 @@
       </c>
       <c r="I73" s="0" t="n">
         <f aca="false">I72+H73</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K73" s="0" t="n">
         <f aca="false">J73-J72</f>
@@ -2186,7 +2246,7 @@
       </c>
       <c r="I74" s="0" t="n">
         <f aca="false">I73+H74</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K74" s="0" t="n">
         <f aca="false">J74-J73</f>
@@ -2207,7 +2267,7 @@
       </c>
       <c r="I75" s="0" t="n">
         <f aca="false">I74+H75</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K75" s="0" t="n">
         <f aca="false">J75-J74</f>
@@ -2228,7 +2288,7 @@
       </c>
       <c r="I76" s="0" t="n">
         <f aca="false">I75+H76</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K76" s="0" t="n">
         <f aca="false">J76-J75</f>
@@ -2249,7 +2309,7 @@
       </c>
       <c r="I77" s="0" t="n">
         <f aca="false">I76+H77</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K77" s="0" t="n">
         <f aca="false">J77-J76</f>
@@ -2270,7 +2330,7 @@
       </c>
       <c r="I78" s="0" t="n">
         <f aca="false">I77+H78</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K78" s="0" t="n">
         <f aca="false">J78-J77</f>
@@ -2291,7 +2351,7 @@
       </c>
       <c r="I79" s="0" t="n">
         <f aca="false">I78+H79</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K79" s="0" t="n">
         <f aca="false">J79-J78</f>
@@ -2312,7 +2372,7 @@
       </c>
       <c r="I80" s="0" t="n">
         <f aca="false">I79+H80</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K80" s="0" t="n">
         <f aca="false">J80-J79</f>
@@ -2333,7 +2393,7 @@
       </c>
       <c r="I81" s="0" t="n">
         <f aca="false">I80+H81</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K81" s="0" t="n">
         <f aca="false">J81-J80</f>
@@ -2354,7 +2414,7 @@
       </c>
       <c r="I82" s="0" t="n">
         <f aca="false">I81+H82</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K82" s="0" t="n">
         <f aca="false">J82-J81</f>
@@ -2375,7 +2435,7 @@
       </c>
       <c r="I83" s="0" t="n">
         <f aca="false">I82+H83</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K83" s="0" t="n">
         <f aca="false">J83-J82</f>
@@ -2396,7 +2456,7 @@
       </c>
       <c r="I84" s="0" t="n">
         <f aca="false">I83+H84</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K84" s="0" t="n">
         <f aca="false">J84-J83</f>
@@ -2417,7 +2477,7 @@
       </c>
       <c r="I85" s="0" t="n">
         <f aca="false">I84+H85</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K85" s="0" t="n">
         <f aca="false">J85-J84</f>
@@ -2438,7 +2498,7 @@
       </c>
       <c r="I86" s="0" t="n">
         <f aca="false">I85+H86</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K86" s="0" t="n">
         <f aca="false">J86-J85</f>
@@ -2459,7 +2519,7 @@
       </c>
       <c r="I87" s="0" t="n">
         <f aca="false">I86+H87</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K87" s="0" t="n">
         <f aca="false">J87-J86</f>
@@ -2480,7 +2540,7 @@
       </c>
       <c r="I88" s="0" t="n">
         <f aca="false">I87+H88</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K88" s="0" t="n">
         <f aca="false">J88-J87</f>
@@ -2501,7 +2561,7 @@
       </c>
       <c r="I89" s="0" t="n">
         <f aca="false">I88+H89</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K89" s="0" t="n">
         <f aca="false">J89-J88</f>
@@ -2522,7 +2582,7 @@
       </c>
       <c r="I90" s="0" t="n">
         <f aca="false">I89+H90</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K90" s="0" t="n">
         <f aca="false">J90-J89</f>
@@ -2543,7 +2603,7 @@
       </c>
       <c r="I91" s="0" t="n">
         <f aca="false">I90+H91</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K91" s="0" t="n">
         <f aca="false">J91-J90</f>
@@ -2564,7 +2624,7 @@
       </c>
       <c r="I92" s="0" t="n">
         <f aca="false">I91+H92</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K92" s="0" t="n">
         <f aca="false">J92-J91</f>
@@ -2585,7 +2645,7 @@
       </c>
       <c r="I93" s="0" t="n">
         <f aca="false">I92+H93</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K93" s="0" t="n">
         <f aca="false">J93-J92</f>
@@ -2606,7 +2666,7 @@
       </c>
       <c r="I94" s="0" t="n">
         <f aca="false">I93+H94</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K94" s="0" t="n">
         <f aca="false">J94-J93</f>
@@ -2627,7 +2687,7 @@
       </c>
       <c r="I95" s="0" t="n">
         <f aca="false">I94+H95</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K95" s="0" t="n">
         <f aca="false">J95-J94</f>
@@ -2648,7 +2708,7 @@
       </c>
       <c r="I96" s="0" t="n">
         <f aca="false">I95+H96</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K96" s="0" t="n">
         <f aca="false">J96-J95</f>
@@ -2669,7 +2729,7 @@
       </c>
       <c r="I97" s="0" t="n">
         <f aca="false">I96+H97</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K97" s="0" t="n">
         <f aca="false">J97-J96</f>
@@ -2690,7 +2750,7 @@
       </c>
       <c r="I98" s="0" t="n">
         <f aca="false">I97+H98</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K98" s="0" t="n">
         <f aca="false">J98-J97</f>
@@ -2711,7 +2771,7 @@
       </c>
       <c r="I99" s="0" t="n">
         <f aca="false">I98+H99</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K99" s="0" t="n">
         <f aca="false">J99-J98</f>
@@ -2732,7 +2792,7 @@
       </c>
       <c r="I100" s="0" t="n">
         <f aca="false">I99+H100</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K100" s="0" t="n">
         <f aca="false">J100-J99</f>
@@ -2753,7 +2813,7 @@
       </c>
       <c r="I101" s="0" t="n">
         <f aca="false">I100+H101</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K101" s="0" t="n">
         <f aca="false">J101-J100</f>
@@ -2774,7 +2834,7 @@
       </c>
       <c r="I102" s="0" t="n">
         <f aca="false">I101+H102</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K102" s="0" t="n">
         <f aca="false">J102-J101</f>
@@ -2795,7 +2855,7 @@
       </c>
       <c r="I103" s="0" t="n">
         <f aca="false">I102+H103</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K103" s="0" t="n">
         <f aca="false">J103-J102</f>
@@ -2816,7 +2876,7 @@
       </c>
       <c r="I104" s="0" t="n">
         <f aca="false">I103+H104</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K104" s="0" t="n">
         <f aca="false">J104-J103</f>
@@ -2837,7 +2897,7 @@
       </c>
       <c r="I105" s="0" t="n">
         <f aca="false">I104+H105</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K105" s="0" t="n">
         <f aca="false">J105-J104</f>
@@ -2858,7 +2918,7 @@
       </c>
       <c r="I106" s="0" t="n">
         <f aca="false">I105+H106</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K106" s="0" t="n">
         <f aca="false">J106-J105</f>
@@ -2879,7 +2939,7 @@
       </c>
       <c r="I107" s="0" t="n">
         <f aca="false">I106+H107</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K107" s="0" t="n">
         <f aca="false">J107-J106</f>
@@ -2900,7 +2960,7 @@
       </c>
       <c r="I108" s="0" t="n">
         <f aca="false">I107+H108</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K108" s="0" t="n">
         <f aca="false">J108-J107</f>
@@ -2921,7 +2981,7 @@
       </c>
       <c r="I109" s="0" t="n">
         <f aca="false">I108+H109</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K109" s="0" t="n">
         <f aca="false">J109-J108</f>
@@ -2942,7 +3002,7 @@
       </c>
       <c r="I110" s="0" t="n">
         <f aca="false">I109+H110</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K110" s="0" t="n">
         <f aca="false">J110-J109</f>
@@ -2963,7 +3023,7 @@
       </c>
       <c r="I111" s="0" t="n">
         <f aca="false">I110+H111</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K111" s="0" t="n">
         <f aca="false">J111-J110</f>
@@ -2984,7 +3044,7 @@
       </c>
       <c r="I112" s="0" t="n">
         <f aca="false">I111+H112</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K112" s="0" t="n">
         <f aca="false">J112-J111</f>
@@ -3005,7 +3065,7 @@
       </c>
       <c r="I113" s="0" t="n">
         <f aca="false">I112+H113</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K113" s="0" t="n">
         <f aca="false">J113-J112</f>
@@ -3026,7 +3086,7 @@
       </c>
       <c r="I114" s="0" t="n">
         <f aca="false">I113+H114</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K114" s="0" t="n">
         <f aca="false">J114-J113</f>
@@ -3047,7 +3107,7 @@
       </c>
       <c r="I115" s="0" t="n">
         <f aca="false">I114+H115</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K115" s="0" t="n">
         <f aca="false">J115-J114</f>
@@ -3068,7 +3128,7 @@
       </c>
       <c r="I116" s="0" t="n">
         <f aca="false">I115+H116</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K116" s="0" t="n">
         <f aca="false">J116-J115</f>
@@ -3089,7 +3149,7 @@
       </c>
       <c r="I117" s="0" t="n">
         <f aca="false">I116+H117</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K117" s="0" t="n">
         <f aca="false">J117-J116</f>
@@ -3110,7 +3170,7 @@
       </c>
       <c r="I118" s="0" t="n">
         <f aca="false">I117+H118</f>
-        <v>2160</v>
+        <v>4057</v>
       </c>
       <c r="K118" s="0" t="n">
         <f aca="false">J118-J117</f>

</xml_diff>